<commit_message>
1474 column without name fixed (#1475)
* 1474 fixed

* var name changed

* building

* correcting .yml
</commit_message>
<xml_diff>
--- a/tests/OSPSuite.Infrastructure.Tests/Data/ExcelImport/psv.xlsx
+++ b/tests/OSPSuite.Infrastructure.Tests/Data/ExcelImport/psv.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58C82197-0839-4E6A-9725-82EC4515FA93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -18,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>Path</t>
   </si>
@@ -87,12 +88,18 @@
   </si>
   <si>
     <t>A|B|H</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,6 +140,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -181,7 +191,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -214,9 +224,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -249,6 +276,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -424,16 +468,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -444,7 +488,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -455,7 +499,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -465,8 +509,11 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -476,8 +523,11 @@
       <c r="C4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -488,7 +538,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -499,7 +549,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -517,16 +567,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -542,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -550,7 +600,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -558,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -566,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -574,7 +624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -588,16 +638,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -608,7 +658,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -619,7 +669,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -630,7 +680,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -641,7 +691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -652,7 +702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -663,7 +713,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -680,16 +730,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -700,7 +750,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -711,7 +761,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -722,7 +772,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -733,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -744,7 +794,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -755,7 +805,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -772,12 +822,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>